<commit_message>
Add bad examples for multiple rules
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
   <si>
     <t>Table 1</t>
   </si>
@@ -295,6 +295,9 @@
     <t>Try/catch Blöcke</t>
   </si>
   <si>
+    <t>HILFE, Erklärung nötig! -&gt; Schlecht, wenn zu großer try block?</t>
+  </si>
+  <si>
     <t>Unspecified Error Message</t>
   </si>
   <si>
@@ -327,12 +330,21 @@
     </r>
   </si>
   <si>
+    <t>UseUtilityClass</t>
+  </si>
+  <si>
     <t>Unsafe Cast</t>
   </si>
   <si>
     <t>Empty Constructor</t>
   </si>
   <si>
+    <t>UnnecessaryConstructor</t>
+  </si>
+  <si>
+    <t>UncommentedEmptyConstructor</t>
+  </si>
+  <si>
     <t>Meaningless constants</t>
   </si>
   <si>
@@ -356,6 +368,9 @@
     </r>
   </si>
   <si>
+    <t>UnusedPrivateMethod</t>
+  </si>
+  <si>
     <t>Unused public methods -&gt; NO RULE EXISTING</t>
   </si>
   <si>
@@ -373,6 +388,9 @@
     </r>
   </si>
   <si>
+    <t>UnusedPrivateField</t>
+  </si>
+  <si>
     <t>Unused local variables should be removed</t>
   </si>
   <si>
@@ -387,6 +405,9 @@
     </r>
   </si>
   <si>
+    <t>UnusedLocalVariable</t>
+  </si>
+  <si>
     <t>Missing `throws` statement in method signature</t>
   </si>
   <si>
@@ -587,6 +608,9 @@
   </si>
   <si>
     <t>Final Modifier</t>
+  </si>
+  <si>
+    <t>Don’t find a perfect solution</t>
   </si>
   <si>
     <t>Assert vs IF</t>
@@ -935,7 +959,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -993,6 +1017,9 @@
     <xf numFmtId="49" fontId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1006,6 +1033,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2095,7 +2125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:E71"/>
+  <dimension ref="A2:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2106,9 +2136,8 @@
     <col min="1" max="1" width="46.4375" style="1" customWidth="1"/>
     <col min="2" max="2" width="71.6953" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.22656" style="1" customWidth="1"/>
-    <col min="4" max="4" width="69.2812" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6562" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5234" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -2118,7 +2147,6 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -2133,9 +2161,6 @@
       <c r="D2" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
-        <v>3</v>
-      </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="4">
@@ -2144,7 +2169,6 @@
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="56.05" customHeight="1">
       <c r="A4" t="s" s="7">
@@ -2155,7 +2179,6 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
       <c r="A5" s="10"/>
@@ -2166,9 +2189,8 @@
         <v>9</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" ht="80.05" customHeight="1">
+    </row>
+    <row r="6" ht="116.05" customHeight="1">
       <c r="A6" t="s" s="7">
         <v>10</v>
       </c>
@@ -2179,7 +2201,6 @@
       <c r="D6" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="E6" s="9"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="7">
@@ -2192,7 +2213,6 @@
         <v>15</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="15">
@@ -2201,7 +2221,6 @@
       <c r="B8" s="16"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="32.05" customHeight="1">
       <c r="A9" t="s" s="7">
@@ -2214,7 +2233,6 @@
         <v>19</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="7">
@@ -2227,7 +2245,6 @@
         <v>22</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="10"/>
@@ -2238,7 +2255,6 @@
         <v>24</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="7">
@@ -2247,7 +2263,6 @@
       <c r="B12" s="16"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
     </row>
     <row r="13" ht="32.05" customHeight="1">
       <c r="A13" t="s" s="17">
@@ -2257,26 +2272,25 @@
         <v>27</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="20">
         <v>28</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
     </row>
     <row r="15" ht="63.2" customHeight="1">
-      <c r="A15" t="s" s="21">
+      <c r="A15" t="s" s="22">
         <v>29</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="7">
@@ -2288,8 +2302,9 @@
       <c r="C16" t="s" s="12">
         <v>32</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="D16" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="7">
@@ -2298,51 +2313,46 @@
       <c r="B17" s="16"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="7">
         <v>34</v>
       </c>
-      <c r="B18" t="s" s="22">
+      <c r="B18" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="7">
         <v>36</v>
       </c>
-      <c r="B19" t="s" s="22">
+      <c r="B19" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="7">
         <v>37</v>
       </c>
-      <c r="B20" t="s" s="22">
+      <c r="B20" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="7">
         <v>38</v>
       </c>
-      <c r="B21" t="s" s="23">
+      <c r="B21" t="s" s="24">
         <v>39</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="7">
@@ -2355,546 +2365,546 @@
         <v>15</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="7">
         <v>40</v>
       </c>
-      <c r="B23" t="s" s="22">
+      <c r="B23" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="7">
         <v>41</v>
       </c>
-      <c r="B24" t="s" s="23">
-        <v>39</v>
+      <c r="B24" t="s" s="24">
+        <v>42</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s" s="22">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s" s="22">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="B27" t="s" s="22">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s" s="22">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s" s="23">
         <v>35</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s" s="14">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s" s="12">
-        <v>49</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="D30" t="s" s="12">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="7">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="D31" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="7">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="D32" t="s" s="12">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" t="s" s="7">
-        <v>52</v>
-      </c>
-      <c r="B33" t="s" s="22">
+      <c r="A33" s="10"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="9"/>
+      <c r="D33" t="s" s="12">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" t="s" s="7">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s" s="23">
         <v>35</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" ht="32.05" customHeight="1">
-      <c r="A34" t="s" s="7">
-        <v>53</v>
-      </c>
-      <c r="B34" s="16"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" ht="20.05" customHeight="1">
+    </row>
+    <row r="35" ht="32.05" customHeight="1">
       <c r="A35" t="s" s="7">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s" s="14">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s" s="12">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
     </row>
     <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" s="10"/>
-      <c r="B36" t="s" s="18">
-        <v>57</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="A36" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s" s="14">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s" s="12">
+        <v>60</v>
+      </c>
+      <c r="D36" t="s" s="12">
+        <v>61</v>
+      </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" s="10"/>
-      <c r="B37" t="s" s="14">
-        <v>58</v>
-      </c>
-      <c r="C37" t="s" s="12">
-        <v>59</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="B37" t="s" s="18">
+        <v>62</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" t="s" s="19">
+        <v>62</v>
+      </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" t="s" s="14">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s" s="12">
-        <v>61</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="D38" t="s" s="12">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s" s="18">
-        <v>27</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="A39" s="10"/>
+      <c r="B39" t="s" s="14">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s" s="12">
+        <v>67</v>
+      </c>
+      <c r="D39" t="s" s="12">
+        <v>68</v>
+      </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="7">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
+      <c r="D40" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="7">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
+      <c r="D41" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="7">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+      <c r="D42" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="7">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" ht="20.35" customHeight="1">
+      <c r="D43" t="s" s="19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="B44" t="s" s="14">
-        <v>68</v>
-      </c>
-      <c r="C44" t="s" s="12">
-        <v>69</v>
-      </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" s="10"/>
+        <v>73</v>
+      </c>
+      <c r="B44" t="s" s="18">
+        <v>27</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" t="s" s="19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" ht="20.35" customHeight="1">
+      <c r="A45" t="s" s="7">
+        <v>74</v>
+      </c>
       <c r="B45" t="s" s="14">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s" s="12">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
     </row>
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" t="s" s="14">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s" s="12">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" t="s" s="14">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s" s="12">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" s="10"/>
       <c r="B48" t="s" s="14">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s" s="12">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" s="10"/>
       <c r="B49" t="s" s="14">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s" s="12">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" s="10"/>
       <c r="B50" t="s" s="14">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s" s="12">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" s="10"/>
       <c r="B51" t="s" s="14">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s" s="12">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" s="10"/>
       <c r="B52" t="s" s="14">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s" s="12">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" s="10"/>
       <c r="B53" t="s" s="14">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s" s="12">
+        <v>92</v>
+      </c>
+      <c r="D53" s="9"/>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" s="10"/>
+      <c r="B54" t="s" s="14">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-    </row>
-    <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" t="s" s="7">
-        <v>87</v>
-      </c>
-      <c r="B54" t="s" s="18">
-        <v>27</v>
-      </c>
-      <c r="C54" s="9"/>
       <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="7">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s" s="18">
         <v>27</v>
       </c>
       <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
+      <c r="D55" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="7">
-        <v>89</v>
-      </c>
-      <c r="B56" t="s" s="22">
-        <v>35</v>
+        <v>95</v>
+      </c>
+      <c r="B56" t="s" s="18">
+        <v>27</v>
       </c>
       <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
+      <c r="D56" t="s" s="19">
+        <v>27</v>
+      </c>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="7">
-        <v>90</v>
-      </c>
-      <c r="B57" t="s" s="18">
-        <v>27</v>
+        <v>96</v>
+      </c>
+      <c r="B57" t="s" s="23">
+        <v>35</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-    </row>
-    <row r="58" ht="32.05" customHeight="1">
+    </row>
+    <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="7">
-        <v>91</v>
-      </c>
-      <c r="B58" t="s" s="14">
-        <v>92</v>
-      </c>
-      <c r="C58" t="s" s="12">
-        <v>93</v>
-      </c>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-    </row>
-    <row r="59" ht="20.05" customHeight="1">
+        <v>97</v>
+      </c>
+      <c r="B58" t="s" s="18">
+        <v>27</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" t="s" s="19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" ht="32.05" customHeight="1">
       <c r="A59" t="s" s="7">
-        <v>94</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="9"/>
+        <v>98</v>
+      </c>
+      <c r="B59" t="s" s="14">
+        <v>99</v>
+      </c>
+      <c r="C59" t="s" s="12">
+        <v>100</v>
+      </c>
       <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
     </row>
     <row r="60" ht="20.05" customHeight="1">
       <c r="A60" t="s" s="7">
-        <v>95</v>
-      </c>
-      <c r="B60" t="s" s="14">
-        <v>21</v>
-      </c>
-      <c r="C60" t="s" s="12">
-        <v>22</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B60" t="s" s="23">
+        <v>102</v>
+      </c>
+      <c r="C60" s="9"/>
       <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-    </row>
-    <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" t="s" s="7">
-        <v>96</v>
-      </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="9"/>
+    </row>
+    <row r="61" ht="32.05" customHeight="1">
+      <c r="A61" s="10"/>
+      <c r="B61" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s" s="12">
+        <v>9</v>
+      </c>
       <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
     </row>
     <row r="62" ht="20.05" customHeight="1">
       <c r="A62" t="s" s="7">
-        <v>97</v>
-      </c>
-      <c r="B62" t="s" s="22">
-        <v>35</v>
-      </c>
-      <c r="C62" s="9"/>
+        <v>103</v>
+      </c>
+      <c r="B62" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s" s="12">
+        <v>22</v>
+      </c>
       <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-    </row>
-    <row r="63" ht="32.05" customHeight="1">
+    </row>
+    <row r="63" ht="20.05" customHeight="1">
       <c r="A63" t="s" s="7">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B63" s="16"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-    </row>
-    <row r="64" ht="32.05" customHeight="1">
+    </row>
+    <row r="64" ht="20.05" customHeight="1">
       <c r="A64" t="s" s="7">
-        <v>99</v>
-      </c>
-      <c r="B64" t="s" s="14">
-        <v>18</v>
-      </c>
-      <c r="C64" t="s" s="12">
-        <v>19</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B64" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="C64" s="9"/>
       <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-    </row>
-    <row r="65" ht="20.05" customHeight="1">
+    </row>
+    <row r="65" ht="32.05" customHeight="1">
       <c r="A65" t="s" s="7">
-        <v>100</v>
-      </c>
-      <c r="B65" t="s" s="22">
-        <v>35</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B65" s="16"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
     </row>
     <row r="66" ht="32.05" customHeight="1">
       <c r="A66" t="s" s="7">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s" s="14">
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="C66" t="s" s="12">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
     </row>
     <row r="67" ht="20.05" customHeight="1">
-      <c r="A67" s="10"/>
-      <c r="B67" t="s" s="14">
-        <v>104</v>
-      </c>
-      <c r="C67" t="s" s="12">
-        <v>105</v>
-      </c>
+      <c r="A67" t="s" s="7">
+        <v>108</v>
+      </c>
+      <c r="B67" t="s" s="23">
+        <v>35</v>
+      </c>
+      <c r="C67" s="9"/>
       <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-    </row>
-    <row r="68" ht="20.05" customHeight="1">
-      <c r="A68" s="10"/>
+    </row>
+    <row r="68" ht="32.05" customHeight="1">
+      <c r="A68" t="s" s="7">
+        <v>109</v>
+      </c>
       <c r="B68" t="s" s="14">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C68" t="s" s="12">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-    </row>
-    <row r="69" ht="32.05" customHeight="1">
-      <c r="A69" t="s" s="7">
-        <v>108</v>
-      </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="9"/>
+    </row>
+    <row r="69" ht="20.05" customHeight="1">
+      <c r="A69" s="10"/>
+      <c r="B69" t="s" s="14">
+        <v>112</v>
+      </c>
+      <c r="C69" t="s" s="12">
+        <v>113</v>
+      </c>
       <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-    </row>
-    <row r="70" ht="32.05" customHeight="1">
-      <c r="A70" t="s" s="7">
-        <v>109</v>
-      </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="9"/>
+    </row>
+    <row r="70" ht="20.05" customHeight="1">
+      <c r="A70" s="10"/>
+      <c r="B70" t="s" s="14">
+        <v>114</v>
+      </c>
+      <c r="C70" t="s" s="12">
+        <v>115</v>
+      </c>
       <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-    </row>
-    <row r="71" ht="20.05" customHeight="1">
-      <c r="A71" s="10"/>
+    </row>
+    <row r="71" ht="32.05" customHeight="1">
+      <c r="A71" t="s" s="7">
+        <v>116</v>
+      </c>
       <c r="B71" s="16"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
+    </row>
+    <row r="72" ht="32.05" customHeight="1">
+      <c r="A72" t="s" s="7">
+        <v>117</v>
+      </c>
+      <c r="B72" s="16"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+    </row>
+    <row r="73" ht="20.05" customHeight="1">
+      <c r="A73" s="10"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="https://rules.sonarsource.com/java"/>
@@ -2907,25 +2917,26 @@
     <hyperlink ref="C16" r:id="rId8" location="" tooltip="" display="4144"/>
     <hyperlink ref="C22" r:id="rId9" location="" tooltip="" display="3740"/>
     <hyperlink ref="C30" r:id="rId10" location="" tooltip="" display="1118"/>
-    <hyperlink ref="C35" r:id="rId11" location="" tooltip="" display="1144"/>
-    <hyperlink ref="C37" r:id="rId12" location="" tooltip="" display="1068"/>
-    <hyperlink ref="C38" r:id="rId13" location="" tooltip="" display="1481"/>
-    <hyperlink ref="C44" r:id="rId14" location="" tooltip="" display="100"/>
-    <hyperlink ref="C45" r:id="rId15" location="" tooltip="" display="101"/>
-    <hyperlink ref="C46" r:id="rId16" location="" tooltip="" display="114"/>
-    <hyperlink ref="C47" r:id="rId17" location="" tooltip="" display="115"/>
-    <hyperlink ref="C48" r:id="rId18" location="" tooltip="" display="116"/>
-    <hyperlink ref="C49" r:id="rId19" location="" tooltip="" display="117"/>
-    <hyperlink ref="C50" r:id="rId20" location="" tooltip="" display="118"/>
-    <hyperlink ref="C51" r:id="rId21" location="" tooltip="" display="119"/>
-    <hyperlink ref="C52" r:id="rId22" location="" tooltip="" display="120"/>
-    <hyperlink ref="C53" r:id="rId23" location="" tooltip="" display="3008"/>
-    <hyperlink ref="C58" r:id="rId24" location="" tooltip="" display="1170"/>
-    <hyperlink ref="C60" r:id="rId25" location="" tooltip="" display="5960"/>
-    <hyperlink ref="C64" r:id="rId26" location="" tooltip="" display="1319"/>
-    <hyperlink ref="C66" r:id="rId27" location="" tooltip="" display="2094"/>
-    <hyperlink ref="C67" r:id="rId28" location="" tooltip="" display="1186"/>
-    <hyperlink ref="C68" r:id="rId29" location="" tooltip="" display="108"/>
+    <hyperlink ref="C36" r:id="rId11" location="" tooltip="" display="1144"/>
+    <hyperlink ref="C38" r:id="rId12" location="" tooltip="" display="1068"/>
+    <hyperlink ref="C39" r:id="rId13" location="" tooltip="" display="1481"/>
+    <hyperlink ref="C45" r:id="rId14" location="" tooltip="" display="100"/>
+    <hyperlink ref="C46" r:id="rId15" location="" tooltip="" display="101"/>
+    <hyperlink ref="C47" r:id="rId16" location="" tooltip="" display="114"/>
+    <hyperlink ref="C48" r:id="rId17" location="" tooltip="" display="115"/>
+    <hyperlink ref="C49" r:id="rId18" location="" tooltip="" display="116"/>
+    <hyperlink ref="C50" r:id="rId19" location="" tooltip="" display="117"/>
+    <hyperlink ref="C51" r:id="rId20" location="" tooltip="" display="118"/>
+    <hyperlink ref="C52" r:id="rId21" location="" tooltip="" display="119"/>
+    <hyperlink ref="C53" r:id="rId22" location="" tooltip="" display="120"/>
+    <hyperlink ref="C54" r:id="rId23" location="" tooltip="" display="3008"/>
+    <hyperlink ref="C59" r:id="rId24" location="" tooltip="" display="1170"/>
+    <hyperlink ref="C61" r:id="rId25" location="" tooltip="" display="3008"/>
+    <hyperlink ref="C62" r:id="rId26" location="" tooltip="" display="5960"/>
+    <hyperlink ref="C66" r:id="rId27" location="" tooltip="" display="1319"/>
+    <hyperlink ref="C68" r:id="rId28" location="" tooltip="" display="2094"/>
+    <hyperlink ref="C69" r:id="rId29" location="" tooltip="" display="1186"/>
+    <hyperlink ref="C70" r:id="rId30" location="" tooltip="" display="108"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>